<commit_message>
Added Unit itests, Tidied up rhodes diagram plots
</commit_message>
<xml_diff>
--- a/Examples/Error_propagation/Cpx_Liq_Error_prop_Feig2010_example.xlsx
+++ b/Examples/Error_propagation/Cpx_Liq_Error_prop_Feig2010_example.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oregonstateuniversity-my.sharepoint.com/personal/wieserp_oregonstate_edu/Documents/Postdoc/PYthonBarometers/ClassicalThermometers_20210114T090546Z_001/ClassicalThermometers/Benchmarking/Clinopyroxene_Benchmarks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\Examples\Error_propagation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E9C66BC-F9E4-484B-B06D-63D10C1BB1D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F6D9E5-E377-4410-8959-CE50E59F3D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{EB6A5B17-6B7D-45D9-8D27-4A36EDEB9306}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -582,7 +582,7 @@
   <dimension ref="A1:BI8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="BE3" sqref="BE3"/>
+      <selection activeCell="BA1" sqref="BA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>